<commit_message>
Readme update and code fixes
</commit_message>
<xml_diff>
--- a/DataDictionaryFinal.xlsx
+++ b/DataDictionaryFinal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DotNet_II\Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DotNet3\FinalProjectReadmeUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D5028D6-1521-4EE2-B4AB-81F0283706D4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5301FC2F-8CD7-4082-8A1C-9D6D83E36439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="672" windowWidth="11256" windowHeight="11688" tabRatio="981" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" tabRatio="981" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -931,29 +931,29 @@
   <dimension ref="A1:O97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.44140625" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" customWidth="1"/>
     <col min="10" max="10" width="8" customWidth="1"/>
-    <col min="11" max="12" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.6640625" customWidth="1"/>
+    <col min="11" max="12" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
         <v>42</v>
       </c>
@@ -1019,7 +1019,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>14</v>
       </c>
@@ -1050,7 +1050,7 @@
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
@@ -1081,7 +1081,7 @@
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
@@ -1112,7 +1112,7 @@
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>29</v>
       </c>
@@ -1143,7 +1143,7 @@
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
         <v>43</v>
       </c>
@@ -1162,7 +1162,7 @@
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>40</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>39</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>80</v>
       </c>
@@ -1257,7 +1257,7 @@
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
@@ -1286,7 +1286,7 @@
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
         <v>44</v>
       </c>
@@ -1305,7 +1305,7 @@
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>15</v>
       </c>
@@ -1336,7 +1336,7 @@
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>25</v>
       </c>
@@ -1365,7 +1365,7 @@
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>12</v>
       </c>
@@ -1394,7 +1394,7 @@
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>29</v>
       </c>
@@ -1425,7 +1425,7 @@
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="25" t="s">
         <v>45</v>
       </c>
@@ -1444,7 +1444,7 @@
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>47</v>
       </c>
@@ -1475,7 +1475,7 @@
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>48</v>
       </c>
@@ -1506,7 +1506,7 @@
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>10</v>
       </c>
@@ -1535,7 +1535,7 @@
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>11</v>
       </c>
@@ -1564,7 +1564,7 @@
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
     </row>
-    <row r="26" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="29" t="s">
         <v>55</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="29" t="s">
         <v>54</v>
       </c>
@@ -1624,7 +1624,7 @@
       <c r="N27" s="29"/>
       <c r="O27" s="29"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="26" t="s">
         <v>49</v>
       </c>
@@ -1643,7 +1643,7 @@
       <c r="N29" s="9"/>
       <c r="O29" s="9"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
         <v>18</v>
       </c>
@@ -1674,7 +1674,7 @@
       <c r="N30" s="10"/>
       <c r="O30" s="10"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>12</v>
       </c>
@@ -1703,7 +1703,7 @@
       <c r="N31" s="10"/>
       <c r="O31" s="10"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>29</v>
       </c>
@@ -1734,7 +1734,7 @@
       <c r="N32" s="10"/>
       <c r="O32" s="10"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="26" t="s">
         <v>50</v>
       </c>
@@ -1753,7 +1753,7 @@
       <c r="N34" s="9"/>
       <c r="O34" s="9"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
         <v>27</v>
       </c>
@@ -1784,7 +1784,7 @@
       <c r="N35" s="10"/>
       <c r="O35" s="10"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>15</v>
       </c>
@@ -1813,7 +1813,7 @@
       </c>
       <c r="O36" s="10"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
         <v>84</v>
       </c>
@@ -1840,7 +1840,7 @@
       <c r="N37" s="10"/>
       <c r="O37" s="10"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
         <v>83</v>
       </c>
@@ -1867,7 +1867,7 @@
       <c r="N38" s="10"/>
       <c r="O38" s="10"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="21" t="s">
         <v>14</v>
       </c>
@@ -1896,7 +1896,7 @@
       </c>
       <c r="O39" s="10"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="26" t="s">
         <v>51</v>
       </c>
@@ -1915,7 +1915,7 @@
       <c r="N41" s="9"/>
       <c r="O41" s="9"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
         <v>19</v>
       </c>
@@ -1946,7 +1946,7 @@
       <c r="N42" s="10"/>
       <c r="O42" s="10"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
         <v>18</v>
       </c>
@@ -1975,7 +1975,7 @@
       </c>
       <c r="O43" s="10"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
         <v>26</v>
       </c>
@@ -2004,7 +2004,7 @@
       <c r="N44" s="10"/>
       <c r="O44" s="10"/>
     </row>
-    <row r="45" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="12" t="s">
         <v>12</v>
       </c>
@@ -2033,7 +2033,7 @@
       <c r="N45" s="10"/>
       <c r="O45" s="10"/>
     </row>
-    <row r="46" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="16" t="s">
         <v>30</v>
       </c>
@@ -2062,7 +2062,7 @@
       <c r="N46" s="10"/>
       <c r="O46" s="10"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" s="27" t="s">
         <v>53</v>
       </c>
@@ -2081,7 +2081,7 @@
       <c r="N48" s="27"/>
       <c r="O48" s="27"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="16" t="s">
         <v>32</v>
       </c>
@@ -2112,7 +2112,7 @@
       <c r="N49" s="16"/>
       <c r="O49" s="16"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="16" t="s">
         <v>10</v>
       </c>
@@ -2141,7 +2141,7 @@
       <c r="N50" s="16"/>
       <c r="O50" s="16"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="16" t="s">
         <v>11</v>
       </c>
@@ -2170,7 +2170,7 @@
       <c r="N51" s="16"/>
       <c r="O51" s="16"/>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="16" t="s">
         <v>48</v>
       </c>
@@ -2201,7 +2201,7 @@
       <c r="N52" s="16"/>
       <c r="O52" s="16"/>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="16" t="s">
         <v>54</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>37</v>
       </c>
       <c r="C53" s="16">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
@@ -2230,7 +2230,7 @@
       <c r="N53" s="16"/>
       <c r="O53" s="16"/>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="16" t="s">
         <v>29</v>
       </c>
@@ -2259,7 +2259,7 @@
       <c r="N54" s="16"/>
       <c r="O54" s="16"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="16" t="s">
         <v>55</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="26" t="s">
         <v>52</v>
       </c>
@@ -2311,7 +2311,7 @@
       <c r="N57" s="9"/>
       <c r="O57" s="9"/>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
         <v>28</v>
       </c>
@@ -2342,7 +2342,7 @@
       <c r="N58" s="10"/>
       <c r="O58" s="10"/>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
         <v>47</v>
       </c>
@@ -2371,7 +2371,7 @@
       </c>
       <c r="O59" s="10"/>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="16" t="s">
         <v>32</v>
       </c>
@@ -2400,7 +2400,7 @@
       </c>
       <c r="O60" s="10"/>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="18" t="s">
         <v>23</v>
       </c>
@@ -2427,7 +2427,7 @@
       <c r="N61" s="10"/>
       <c r="O61" s="10"/>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="18" t="s">
         <v>16</v>
       </c>
@@ -2456,7 +2456,7 @@
       </c>
       <c r="O62" s="10"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" s="18" t="s">
         <v>17</v>
       </c>
@@ -2485,7 +2485,7 @@
       </c>
       <c r="O63" s="10"/>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" s="16" t="s">
         <v>29</v>
       </c>
@@ -2514,7 +2514,7 @@
       <c r="N64" s="10"/>
       <c r="O64" s="10"/>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" s="26" t="s">
         <v>56</v>
       </c>
@@ -2533,7 +2533,7 @@
       <c r="N66" s="9"/>
       <c r="O66" s="9"/>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" s="18" t="s">
         <v>19</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" s="18" t="s">
         <v>28</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" s="27" t="s">
         <v>68</v>
       </c>
@@ -2618,7 +2618,7 @@
       <c r="N70" s="27"/>
       <c r="O70" s="27"/>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" s="16" t="s">
         <v>66</v>
       </c>
@@ -2647,7 +2647,7 @@
       <c r="N71" s="16"/>
       <c r="O71" s="16"/>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" s="16" t="s">
         <v>15</v>
       </c>
@@ -2672,7 +2672,7 @@
       </c>
       <c r="O72" s="16"/>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" s="27" t="s">
         <v>65</v>
       </c>
@@ -2691,7 +2691,7 @@
       <c r="N74" s="27"/>
       <c r="O74" s="27"/>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" s="16" t="s">
         <v>18</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" s="16" t="s">
         <v>66</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" s="27" t="s">
         <v>72</v>
       </c>
@@ -2772,7 +2772,7 @@
       <c r="N78" s="27"/>
       <c r="O78" s="27"/>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79" s="21" t="s">
         <v>70</v>
       </c>
@@ -2801,7 +2801,7 @@
       <c r="N79" s="21"/>
       <c r="O79" s="21"/>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80" s="16" t="s">
         <v>15</v>
       </c>
@@ -2830,7 +2830,7 @@
       </c>
       <c r="O80" s="16"/>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" s="27" t="s">
         <v>69</v>
       </c>
@@ -2849,7 +2849,7 @@
       <c r="N82" s="27"/>
       <c r="O82" s="27"/>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" s="16" t="s">
         <v>32</v>
       </c>
@@ -2878,7 +2878,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84" s="16" t="s">
         <v>70</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86" s="27" t="s">
         <v>73</v>
       </c>
@@ -2926,7 +2926,7 @@
       <c r="N86" s="27"/>
       <c r="O86" s="27"/>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" s="21" t="s">
         <v>46</v>
       </c>
@@ -2955,7 +2955,7 @@
       <c r="N87" s="21"/>
       <c r="O87" s="21"/>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A88" s="21" t="s">
         <v>47</v>
       </c>
@@ -2982,7 +2982,7 @@
       <c r="N88" s="21"/>
       <c r="O88" s="21"/>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89" s="16" t="s">
         <v>12</v>
       </c>
@@ -3011,7 +3011,7 @@
       <c r="N89" s="16"/>
       <c r="O89" s="16"/>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91" s="27" t="s">
         <v>74</v>
       </c>
@@ -3030,7 +3030,7 @@
       <c r="N91" s="27"/>
       <c r="O91" s="27"/>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92" s="21" t="s">
         <v>76</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" s="16" t="s">
         <v>12</v>
       </c>
@@ -3086,7 +3086,7 @@
       <c r="N93" s="16"/>
       <c r="O93" s="16"/>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" s="27" t="s">
         <v>75</v>
       </c>
@@ -3105,7 +3105,7 @@
       <c r="N95" s="27"/>
       <c r="O95" s="27"/>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" s="21" t="s">
         <v>32</v>
       </c>
@@ -3134,7 +3134,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97" s="16" t="s">
         <v>76</v>
       </c>

</xml_diff>